<commit_message>
Average loops, resized average loops, scaling for all chromosomes in both organisms
1) New classes for parsing & loop utils
2) Refactored utils code
3) Less logic in notebook
4) Average loops for all chromosomes
5) Scaling for all chromosomes
6) Mean average loops, resized average loops and scaling for all chromosomes in both organisms
</commit_message>
<xml_diff>
--- a/dicty/dicty_loop_positions_Chr1_Chr5_Chr6.xlsx
+++ b/dicty/dicty_loop_positions_Chr1_Chr5_Chr6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/ws/hse/diploma/loops/dicty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5A787C-ED60-3643-8A40-40E57A5DD9DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445A9B3C-E64D-5A49-AF9D-962B32464CD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7460" yWindow="460" windowWidth="14200" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loops" sheetId="1" r:id="rId1"/>
@@ -28,15 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>Chr</t>
-  </si>
-  <si>
-    <t>Size (Kb)</t>
   </si>
   <si>
     <t>Chr1_loop bases</t>
@@ -45,19 +42,28 @@
     <t>Chr6_loop bases</t>
   </si>
   <si>
-    <t>"Extrusion track"</t>
-  </si>
-  <si>
-    <t>Genomic bin, Right base</t>
-  </si>
-  <si>
-    <t>Genomic bin, Left base</t>
-  </si>
-  <si>
     <t>Note for extrusion tracks: 0=n/a, 1=from the left base, 2=from the right base</t>
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>chr</t>
+  </si>
+  <si>
+    <t>extrusion_track</t>
   </si>
 </sst>
 </file>
@@ -427,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A407" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D447" sqref="D447"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,25 +451,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,7 +9579,7 @@
         <v>2496</v>
       </c>
       <c r="E435" s="2">
-        <f t="shared" ref="E435:E498" si="7">(D435-C435+1)*2</f>
+        <f t="shared" ref="E435:E438" si="7">(D435-C435+1)*2</f>
         <v>16</v>
       </c>
       <c r="F435" s="2">
@@ -9670,7 +9676,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -9762,10 +9768,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>